<commit_message>
docs: Update .xlsx file and double-checked points
</commit_message>
<xml_diff>
--- a/Informatyka_StrekowskiHubert208381_2.xlsx
+++ b/Informatyka_StrekowskiHubert208381_2.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\PG\HiH\Projekt\202223\Projekt 2\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="10728" yWindow="-48" windowWidth="9828" windowHeight="9480"/>
+    <workbookView xWindow="10725" yWindow="-45" windowWidth="9825" windowHeight="9480"/>
   </bookViews>
   <sheets>
     <sheet name="2 projekt" sheetId="4" r:id="rId1"/>
@@ -17,7 +12,7 @@
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">'2 projekt'!$A$2:$D$34</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -491,9 +486,6 @@
     <t>realizacja</t>
   </si>
   <si>
-    <t>Tutaj wpisać: Imię, nazwisko, nr indeksu</t>
-  </si>
-  <si>
     <t xml:space="preserve">suma XSLT </t>
   </si>
   <si>
@@ -776,12 +768,15 @@
       </rPr>
       <t>dowolnego znacznika lub atrybutu z pliku XML. Nazwa ta ma być pobierana z pliku XML.</t>
     </r>
+  </si>
+  <si>
+    <t>Hubert Strękowski 208381</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0;\-0;;@"/>
   </numFmts>
@@ -971,9 +966,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1073,6 +1065,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
       <alignment wrapText="1"/>
       <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1139,7 +1134,7 @@
     </a:clrScheme>
     <a:fontScheme name="Pakiet Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1171,10 +1166,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1206,7 +1200,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Pakiet Office">
@@ -1382,522 +1375,522 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="79.44140625" style="35" customWidth="1"/>
-    <col min="2" max="2" width="6" style="27" customWidth="1"/>
-    <col min="3" max="3" width="10.21875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="7.44140625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="8.88671875" style="2"/>
-    <col min="6" max="6" width="52.88671875" style="2" customWidth="1"/>
-    <col min="7" max="16384" width="8.88671875" style="2"/>
+    <col min="1" max="1" width="79.42578125" style="34" customWidth="1"/>
+    <col min="2" max="2" width="6" style="26" customWidth="1"/>
+    <col min="3" max="3" width="10.28515625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="7.42578125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="8.85546875" style="2"/>
+    <col min="6" max="6" width="52.85546875" style="2" customWidth="1"/>
+    <col min="7" max="16384" width="8.85546875" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="45" customHeight="1">
-      <c r="A1" s="26" t="s">
-        <v>24</v>
+      <c r="A1" s="25" t="s">
+        <v>37</v>
       </c>
       <c r="B1" s="3"/>
-      <c r="C1" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-    </row>
-    <row r="2" spans="1:6" ht="15">
-      <c r="A2" s="5" t="s">
+      <c r="C1" s="35" t="s">
+        <v>33</v>
+      </c>
+      <c r="D1" s="35"/>
+      <c r="E1" s="35"/>
+      <c r="F1" s="35"/>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="D2" s="7"/>
+      <c r="D2" s="6"/>
     </row>
     <row r="3" spans="1:6" ht="30">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="6">
+      <c r="B3" s="5">
         <v>1.6</v>
       </c>
-      <c r="C3" s="28">
-        <v>1</v>
-      </c>
-      <c r="D3" s="7">
+      <c r="C3" s="27">
+        <v>1</v>
+      </c>
+      <c r="D3" s="6">
         <f>B3*C3</f>
         <v>1.6</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="15">
-      <c r="A4" s="8" t="s">
+    <row r="4" spans="1:6">
+      <c r="A4" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="9">
+      <c r="B4" s="8">
         <v>0.5</v>
       </c>
-      <c r="C4" s="28">
-        <v>1</v>
-      </c>
-      <c r="D4" s="7">
+      <c r="C4" s="27">
+        <v>1</v>
+      </c>
+      <c r="D4" s="6">
         <f t="shared" ref="D4:D15" si="0">B4*C4</f>
         <v>0.5</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="15">
-      <c r="A5" s="8" t="s">
+    <row r="5" spans="1:6">
+      <c r="A5" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="9">
+      <c r="B5" s="8">
         <v>0.5</v>
       </c>
-      <c r="C5" s="28">
-        <v>1</v>
-      </c>
-      <c r="D5" s="7">
+      <c r="C5" s="27">
+        <v>1</v>
+      </c>
+      <c r="D5" s="6">
         <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="15">
-      <c r="A6" s="8" t="s">
+    <row r="6" spans="1:6">
+      <c r="A6" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="9">
+      <c r="B6" s="8">
         <v>0.9</v>
       </c>
-      <c r="C6" s="28">
-        <v>1</v>
-      </c>
-      <c r="D6" s="7">
+      <c r="C6" s="27">
+        <v>1</v>
+      </c>
+      <c r="D6" s="6">
         <f t="shared" si="0"/>
         <v>0.9</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="15">
-      <c r="A7" s="8" t="s">
+    <row r="7" spans="1:6">
+      <c r="A7" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="9">
+      <c r="B7" s="8">
         <v>0.8</v>
       </c>
-      <c r="C7" s="28">
-        <v>1</v>
-      </c>
-      <c r="D7" s="7">
+      <c r="C7" s="27">
+        <v>1</v>
+      </c>
+      <c r="D7" s="6">
         <f t="shared" si="0"/>
         <v>0.8</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="30">
-      <c r="A8" s="8" t="s">
+      <c r="A8" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="9">
-        <v>1</v>
-      </c>
-      <c r="C8" s="28">
-        <v>1</v>
-      </c>
-      <c r="D8" s="7">
+      <c r="B8" s="8">
+        <v>1</v>
+      </c>
+      <c r="C8" s="27">
+        <v>1</v>
+      </c>
+      <c r="D8" s="6">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="45">
-      <c r="A9" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="B9" s="9">
-        <v>1</v>
-      </c>
-      <c r="C9" s="28">
-        <v>1</v>
-      </c>
-      <c r="D9" s="7">
+      <c r="A9" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="B9" s="8">
+        <v>1</v>
+      </c>
+      <c r="C9" s="27">
+        <v>1</v>
+      </c>
+      <c r="D9" s="6">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="15">
-      <c r="A10" s="8" t="s">
+    <row r="10" spans="1:6">
+      <c r="A10" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="B10" s="9">
-        <v>1</v>
-      </c>
-      <c r="C10" s="28">
-        <v>1</v>
-      </c>
-      <c r="D10" s="7">
+      <c r="B10" s="8">
+        <v>1</v>
+      </c>
+      <c r="C10" s="27">
+        <v>1</v>
+      </c>
+      <c r="D10" s="6">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="15">
-      <c r="A11" s="8" t="s">
+    <row r="11" spans="1:6">
+      <c r="A11" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="B11" s="9">
+      <c r="B11" s="8">
         <v>0.8</v>
       </c>
-      <c r="C11" s="28">
-        <v>1</v>
-      </c>
-      <c r="D11" s="7">
+      <c r="C11" s="27">
+        <v>1</v>
+      </c>
+      <c r="D11" s="6">
         <f t="shared" si="0"/>
         <v>0.8</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="15">
-      <c r="A12" s="8" t="s">
+    <row r="12" spans="1:6">
+      <c r="A12" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="9">
+      <c r="B12" s="8">
         <v>0.3</v>
       </c>
-      <c r="C12" s="28">
-        <v>1</v>
-      </c>
-      <c r="D12" s="7">
+      <c r="C12" s="27">
+        <v>1</v>
+      </c>
+      <c r="D12" s="6">
         <f t="shared" si="0"/>
         <v>0.3</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="15">
-      <c r="A13" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="B13" s="6">
+    <row r="13" spans="1:6">
+      <c r="A13" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="B13" s="5">
         <v>0.6</v>
       </c>
-      <c r="C13" s="28">
-        <v>1</v>
-      </c>
-      <c r="D13" s="7">
+      <c r="C13" s="27">
+        <v>1</v>
+      </c>
+      <c r="D13" s="6">
         <f t="shared" si="0"/>
         <v>0.6</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="15">
-      <c r="A14" s="8" t="s">
+    <row r="14" spans="1:6">
+      <c r="A14" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="B14" s="9">
+      <c r="B14" s="8">
         <v>0.8</v>
       </c>
-      <c r="C14" s="28">
-        <v>1</v>
-      </c>
-      <c r="D14" s="7">
+      <c r="C14" s="27">
+        <v>1</v>
+      </c>
+      <c r="D14" s="6">
         <f t="shared" si="0"/>
         <v>0.8</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="15">
-      <c r="A15" s="8" t="s">
+    <row r="15" spans="1:6">
+      <c r="A15" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="B15" s="9">
+      <c r="B15" s="8">
         <v>0.8</v>
       </c>
-      <c r="C15" s="28">
-        <v>1</v>
-      </c>
-      <c r="D15" s="7">
+      <c r="C15" s="27">
+        <v>1</v>
+      </c>
+      <c r="D15" s="6">
         <f t="shared" si="0"/>
         <v>0.8</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="15">
-      <c r="A16" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="B16" s="12">
+    <row r="16" spans="1:6">
+      <c r="A16" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="B16" s="11">
         <f>SUM(B3:B15)</f>
         <v>10.600000000000001</v>
       </c>
-      <c r="C16" s="29"/>
-      <c r="D16" s="12">
+      <c r="C16" s="28"/>
+      <c r="D16" s="11">
         <f>SUM(D3:D15)</f>
         <v>10.600000000000001</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="15">
-      <c r="A17" s="5"/>
-      <c r="B17" s="13"/>
-      <c r="C17" s="30"/>
-      <c r="D17" s="13"/>
-    </row>
-    <row r="18" spans="1:4" ht="15">
-      <c r="A18" s="5" t="s">
+    <row r="17" spans="1:4">
+      <c r="A17" s="4"/>
+      <c r="B17" s="12"/>
+      <c r="C17" s="29"/>
+      <c r="D17" s="12"/>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B18" s="6"/>
-      <c r="C18" s="28"/>
-      <c r="D18" s="7"/>
-    </row>
-    <row r="19" spans="1:4" ht="15">
-      <c r="A19" s="8" t="s">
+      <c r="B18" s="5"/>
+      <c r="C18" s="27"/>
+      <c r="D18" s="6"/>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="B19" s="9">
+      <c r="B19" s="8">
         <v>0.4</v>
       </c>
-      <c r="C19" s="28">
-        <v>1</v>
-      </c>
-      <c r="D19" s="7">
+      <c r="C19" s="27">
+        <v>1</v>
+      </c>
+      <c r="D19" s="6">
         <f t="shared" ref="D19:D27" si="1">B19*C19</f>
         <v>0.4</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="30">
-      <c r="A20" s="8" t="s">
+      <c r="A20" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="B20" s="9">
+      <c r="B20" s="8">
         <v>0.4</v>
       </c>
-      <c r="C20" s="28">
-        <v>1</v>
-      </c>
-      <c r="D20" s="7">
+      <c r="C20" s="27">
+        <v>1</v>
+      </c>
+      <c r="D20" s="6">
         <f t="shared" si="1"/>
         <v>0.4</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="30">
-      <c r="A21" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="B21" s="9">
+      <c r="A21" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="B21" s="8">
         <v>0.4</v>
       </c>
-      <c r="C21" s="28">
-        <v>1</v>
-      </c>
-      <c r="D21" s="7">
+      <c r="C21" s="27">
+        <v>1</v>
+      </c>
+      <c r="D21" s="6">
         <f t="shared" ref="D21" si="2">B21*C21</f>
         <v>0.4</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="30">
-      <c r="A22" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="B22" s="6">
+      <c r="A22" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="B22" s="5">
         <v>0.8</v>
       </c>
-      <c r="C22" s="28">
-        <v>1</v>
-      </c>
-      <c r="D22" s="7">
+      <c r="C22" s="27">
+        <v>1</v>
+      </c>
+      <c r="D22" s="6">
         <f t="shared" si="1"/>
         <v>0.8</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="30">
-      <c r="A23" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="B23" s="6">
+      <c r="A23" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="B23" s="5">
         <v>0.8</v>
       </c>
-      <c r="C23" s="28">
-        <v>1</v>
-      </c>
-      <c r="D23" s="7">
+      <c r="C23" s="27">
+        <v>1</v>
+      </c>
+      <c r="D23" s="6">
         <f t="shared" si="1"/>
         <v>0.8</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="15">
-      <c r="A24" s="14" t="s">
+    <row r="24" spans="1:4">
+      <c r="A24" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="B24" s="9">
+      <c r="B24" s="8">
         <v>0.4</v>
       </c>
-      <c r="C24" s="28">
-        <v>1</v>
-      </c>
-      <c r="D24" s="7">
+      <c r="C24" s="27">
+        <v>1</v>
+      </c>
+      <c r="D24" s="6">
         <f t="shared" si="1"/>
         <v>0.4</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="15">
-      <c r="A25" s="14" t="s">
+    <row r="25" spans="1:4">
+      <c r="A25" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="B25" s="9">
+      <c r="B25" s="8">
         <v>0.4</v>
       </c>
-      <c r="C25" s="28">
-        <v>1</v>
-      </c>
-      <c r="D25" s="7">
+      <c r="C25" s="27">
+        <v>1</v>
+      </c>
+      <c r="D25" s="6">
         <f t="shared" si="1"/>
         <v>0.4</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="15">
-      <c r="A26" s="14" t="s">
+    <row r="26" spans="1:4">
+      <c r="A26" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="B26" s="9">
+      <c r="B26" s="8">
         <v>0.4</v>
       </c>
-      <c r="C26" s="28">
-        <v>1</v>
-      </c>
-      <c r="D26" s="7">
+      <c r="C26" s="27">
+        <v>1</v>
+      </c>
+      <c r="D26" s="6">
         <f t="shared" si="1"/>
         <v>0.4</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="15">
-      <c r="A27" s="14" t="s">
+    <row r="27" spans="1:4">
+      <c r="A27" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="B27" s="9">
+      <c r="B27" s="8">
         <v>0.4</v>
       </c>
-      <c r="C27" s="28">
-        <v>1</v>
-      </c>
-      <c r="D27" s="7">
+      <c r="C27" s="27">
+        <v>1</v>
+      </c>
+      <c r="D27" s="6">
         <f t="shared" si="1"/>
         <v>0.4</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="15">
-      <c r="A28" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="B28" s="15">
+    <row r="28" spans="1:4">
+      <c r="A28" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="B28" s="14">
         <f>SUM(B19:B27)</f>
         <v>4.3999999999999995</v>
       </c>
-      <c r="C28" s="29"/>
-      <c r="D28" s="15">
+      <c r="C28" s="28"/>
+      <c r="D28" s="14">
         <f>SUM(D19:D27)</f>
         <v>4.3999999999999995</v>
       </c>
     </row>
-    <row r="29" spans="1:4" s="32" customFormat="1">
-      <c r="A29" s="16" t="s">
+    <row r="29" spans="1:4" s="31" customFormat="1">
+      <c r="A29" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="B29" s="15">
+      <c r="B29" s="14">
         <f>B28+B16</f>
         <v>15</v>
       </c>
-      <c r="C29" s="31"/>
-      <c r="D29" s="15">
+      <c r="C29" s="30"/>
+      <c r="D29" s="14">
         <f>D28+D16</f>
         <v>15</v>
       </c>
     </row>
     <row r="30" spans="1:4">
-      <c r="A30" s="17" t="s">
+      <c r="A30" s="16" t="s">
         <v>2</v>
       </c>
       <c r="B30" s="3"/>
     </row>
     <row r="31" spans="1:4">
-      <c r="A31" s="25"/>
+      <c r="A31" s="24"/>
       <c r="B31" s="3"/>
     </row>
-    <row r="32" spans="1:4" ht="15.6">
-      <c r="A32" s="19" t="s">
+    <row r="32" spans="1:4" ht="15.75">
+      <c r="A32" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="B32" s="19">
+        <v>-2</v>
+      </c>
+      <c r="C32" s="27"/>
+      <c r="D32" s="32">
+        <f t="shared" ref="D32:D35" si="3">B32*C32</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="15.75">
+      <c r="A33" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="B32" s="20">
+      <c r="B33" s="19">
         <v>-2</v>
       </c>
-      <c r="C32" s="28"/>
-      <c r="D32" s="33">
-        <f t="shared" ref="D32:D36" si="3">B32*C32</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" ht="15.6">
-      <c r="A33" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="B33" s="20">
-        <v>-2</v>
-      </c>
-      <c r="C33" s="28"/>
-      <c r="D33" s="33">
+      <c r="C33" s="27"/>
+      <c r="D33" s="32">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="15.6">
-      <c r="A34" s="19" t="s">
-        <v>29</v>
-      </c>
-      <c r="B34" s="20">
+    <row r="34" spans="1:4" ht="15.75">
+      <c r="A34" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="B34" s="19">
         <v>-1</v>
       </c>
-      <c r="C34" s="28"/>
-      <c r="D34" s="33">
+      <c r="C34" s="27"/>
+      <c r="D34" s="32">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="15.6">
-      <c r="A35" s="19" t="s">
-        <v>32</v>
-      </c>
-      <c r="B35" s="20">
+    <row r="35" spans="1:4" ht="15.75">
+      <c r="A35" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="B35" s="19">
         <v>-2</v>
       </c>
-      <c r="C35" s="28"/>
-      <c r="D35" s="33">
+      <c r="C35" s="27"/>
+      <c r="D35" s="32">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="36" spans="1:4">
-      <c r="A36" s="21" t="s">
-        <v>33</v>
-      </c>
-      <c r="B36" s="6">
+      <c r="A36" s="20" t="s">
+        <v>32</v>
+      </c>
+      <c r="B36" s="5">
         <v>-2</v>
       </c>
-      <c r="C36" s="28"/>
-      <c r="D36" s="28"/>
-    </row>
-    <row r="37" spans="1:4" ht="36.6">
-      <c r="A37" s="22" t="s">
-        <v>1</v>
-      </c>
-      <c r="B37" s="23"/>
-      <c r="C37" s="34"/>
-      <c r="D37" s="24">
+      <c r="C36" s="27"/>
+      <c r="D36" s="27"/>
+    </row>
+    <row r="37" spans="1:4" ht="36">
+      <c r="A37" s="21" t="s">
+        <v>1</v>
+      </c>
+      <c r="B37" s="22"/>
+      <c r="C37" s="33"/>
+      <c r="D37" s="23">
         <f>D29+D32+D33+D34+D35+D30</f>
         <v>15</v>
       </c>
     </row>
     <row r="38" spans="1:4">
-      <c r="D38" s="18"/>
+      <c r="D38" s="17"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="dyi6YkylR6htFAXFvakYunZVVJkS/U6pIzfle6QGa+mUHmEOMUuZH/G66eLlZPqvukmqmY0Gh9l4oWM+JVshyw==" saltValue="QsdZQP4fAG6AYk9TCL9Shw==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="1">
     <mergeCell ref="C1:F1"/>
   </mergeCells>

</xml_diff>